<commit_message>
fix: ajustando a velocidade
</commit_message>
<xml_diff>
--- a/PRJ-23/Resultados/Diagrama_Vn_Completo.xlsx
+++ b/PRJ-23/Resultados/Diagrama_Vn_Completo.xlsx
@@ -468,19 +468,19 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>445141.4376826826</v>
+        <v>434376.4019098243</v>
       </c>
       <c r="C2">
         <v>1.225000018124288</v>
       </c>
       <c r="D2">
-        <v>4760.870991258637</v>
+        <v>4117.311866443833</v>
       </c>
       <c r="E2">
-        <v>77.27690476837331</v>
+        <v>71.86433215499773</v>
       </c>
       <c r="F2">
-        <v>122.1855147979931</v>
+        <v>113.6274860683347</v>
       </c>
       <c r="G2">
         <v>221.36</v>
@@ -489,16 +489,16 @@
         <v>276.7</v>
       </c>
       <c r="I2">
-        <v>28.66200752429337</v>
+        <v>26.39996022013026</v>
       </c>
       <c r="J2">
-        <v>0.7426700734147181</v>
+        <v>0.7328704778298667</v>
       </c>
       <c r="K2">
-        <v>2.656807902931046</v>
+        <v>3.031545613680756</v>
       </c>
       <c r="L2">
-        <v>1.660504939331904</v>
+        <v>1.894716008550473</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -506,19 +506,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>341334.2239359862</v>
+        <v>351110.32440492</v>
       </c>
       <c r="C3">
         <v>1.225000018124288</v>
       </c>
       <c r="D3">
-        <v>3650.633411080066</v>
+        <v>3328.059946966066</v>
       </c>
       <c r="E3">
-        <v>67.6691348559994</v>
+        <v>64.61034829962428</v>
       </c>
       <c r="F3">
-        <v>106.9942967190242</v>
+        <v>102.1579305218</v>
       </c>
       <c r="G3">
         <v>221.36</v>
@@ -527,16 +527,16 @@
         <v>276.7</v>
       </c>
       <c r="I3">
-        <v>21.97801252941561</v>
+        <v>21.33932358298599</v>
       </c>
       <c r="J3">
-        <v>0.709019801388737</v>
+        <v>0.7049204794757324</v>
       </c>
       <c r="K3">
-        <v>3.307811736380903</v>
+        <v>3.607444275370693</v>
       </c>
       <c r="L3">
-        <v>2.067382335238065</v>
+        <v>2.254652672106683</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -550,13 +550,13 @@
         <v>0.3804553170855409</v>
       </c>
       <c r="D4">
-        <v>4099.362930481284</v>
+        <v>3633.084682464455</v>
       </c>
       <c r="E4">
-        <v>128.6710708546156</v>
+        <v>121.1324471307076</v>
       </c>
       <c r="F4">
-        <v>203.4468264367468</v>
+        <v>191.5272157414821</v>
       </c>
       <c r="G4">
         <v>221.36</v>
@@ -565,16 +565,16 @@
         <v>276.7</v>
       </c>
       <c r="I4">
-        <v>79.46373957119891</v>
+        <v>75.0062523101635</v>
       </c>
       <c r="J4">
-        <v>0.8249764719726367</v>
+        <v>0.8219223302565979</v>
       </c>
       <c r="K4">
-        <v>1.064494445931747</v>
+        <v>1.19666741498567</v>
       </c>
       <c r="L4">
-        <v>0.6653090287073419</v>
+        <v>0.7479171343660437</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -588,13 +588,13 @@
         <v>0.9047731467868786</v>
       </c>
       <c r="D5">
-        <v>4099.362930481284</v>
+        <v>3633.084682464455</v>
       </c>
       <c r="E5">
-        <v>83.43780933149206</v>
+        <v>78.54932705867407</v>
       </c>
       <c r="F5">
-        <v>131.926760231183</v>
+        <v>124.1973910894523</v>
       </c>
       <c r="G5">
         <v>221.36</v>
@@ -603,16 +603,16 @@
         <v>276.7</v>
       </c>
       <c r="I5">
-        <v>33.41434517892985</v>
+        <v>31.53998060994971</v>
       </c>
       <c r="J5">
-        <v>0.7595278603204074</v>
+        <v>0.7533984132787424</v>
       </c>
       <c r="K5">
-        <v>2.33067431653355</v>
+        <v>2.608575622681944</v>
       </c>
       <c r="L5">
-        <v>1.456671447833469</v>
+        <v>1.630359764176216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>